<commit_message>
Primer commit de apache poi
</commit_message>
<xml_diff>
--- a/poi-generated-file.xlsx
+++ b/poi-generated-file.xlsx
@@ -26,19 +26,19 @@
     <t>Salary</t>
   </si>
   <si>
-    <t>Rajeev Singh</t>
+    <t>Hola</t>
   </si>
   <si>
     <t>rajeev@example.com</t>
   </si>
   <si>
-    <t>Thomas cook</t>
+    <t>Hola2</t>
   </si>
   <si>
     <t>thomas@example.com</t>
   </si>
   <si>
-    <t>Steve Maiden</t>
+    <t>Hola3</t>
   </si>
   <si>
     <t>steve@example.com</t>
@@ -102,10 +102,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="13.65625" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="21.90234375" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="17.1484375" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="9.15625" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="8.25390625" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="21.7109375" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="16.640625" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="8.8046875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -130,7 +130,7 @@
         <v>5</v>
       </c>
       <c r="C2" t="n" s="2">
-        <v>33837.42171271991</v>
+        <v>33837.77426986111</v>
       </c>
       <c r="D2" t="n">
         <v>1200000.0</v>
@@ -144,7 +144,7 @@
         <v>7</v>
       </c>
       <c r="C3" t="n" s="2">
-        <v>24061.421712719908</v>
+        <v>24061.77426986111</v>
       </c>
       <c r="D3" t="n">
         <v>1500000.0</v>
@@ -158,7 +158,7 @@
         <v>9</v>
       </c>
       <c r="C4" t="n" s="2">
-        <v>31915.421712719908</v>
+        <v>31915.77426986111</v>
       </c>
       <c r="D4" t="n">
         <v>1800000.0</v>

</xml_diff>

<commit_message>
Cambiar apache poi a la version 4.1.1 y en ExcelReader se cambió getCellTypeEnum por getCellType por deprecation
</commit_message>
<xml_diff>
--- a/poi-generated-file.xlsx
+++ b/poi-generated-file.xlsx
@@ -6,7 +6,7 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Employee" r:id="rId3" sheetId="1"/>
+    <sheet name="Employees" r:id="rId3" sheetId="1"/>
   </sheets>
 </workbook>
 </file>
@@ -26,19 +26,19 @@
     <t>Salary</t>
   </si>
   <si>
-    <t>Hola</t>
+    <t>Uno</t>
   </si>
   <si>
     <t>rajeev@example.com</t>
   </si>
   <si>
-    <t>Hola2</t>
+    <t>Dos</t>
   </si>
   <si>
     <t>thomas@example.com</t>
   </si>
   <si>
-    <t>Hola3</t>
+    <t>Tres</t>
   </si>
   <si>
     <t>steve@example.com</t>
@@ -96,16 +96,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="8.25390625" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="8.2578125" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="21.7109375" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="16.640625" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="8.8046875" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="16.64453125" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="8.80859375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -130,7 +130,7 @@
         <v>5</v>
       </c>
       <c r="C2" t="n" s="2">
-        <v>33837.77426986111</v>
+        <v>33837.90597678241</v>
       </c>
       <c r="D2" t="n">
         <v>1200000.0</v>
@@ -144,7 +144,7 @@
         <v>7</v>
       </c>
       <c r="C3" t="n" s="2">
-        <v>24061.77426986111</v>
+        <v>24061.905976782407</v>
       </c>
       <c r="D3" t="n">
         <v>1500000.0</v>
@@ -158,7 +158,7 @@
         <v>9</v>
       </c>
       <c r="C4" t="n" s="2">
-        <v>31915.77426986111</v>
+        <v>31915.905976782407</v>
       </c>
       <c r="D4" t="n">
         <v>1800000.0</v>

</xml_diff>